<commit_message>
SL saldo gc e salvataggio
</commit_message>
<xml_diff>
--- a/processed/altre_entrate_tot_tab_budget_fin.xlsx
+++ b/processed/altre_entrate_tot_tab_budget_fin.xlsx
@@ -440,40 +440,40 @@
         <v>13</v>
       </c>
       <c r="B2" t="n">
-        <v>0.658293317089377</v>
+        <v>4016941.7114761</v>
       </c>
       <c r="C2" t="n">
-        <v>0.670701287270711</v>
+        <v>4103861.03807255</v>
       </c>
       <c r="D2" t="n">
-        <v>0.924373974560953</v>
+        <v>3929571.13047073</v>
       </c>
       <c r="E2" t="n">
-        <v>0.646246784117853</v>
+        <v>3652551.91152812</v>
       </c>
       <c r="F2" t="n">
-        <v>0.665827028609072</v>
+        <v>3943910.75973798</v>
       </c>
       <c r="G2" t="n">
-        <v>0.706129495536736</v>
+        <v>4846787.73915926</v>
       </c>
       <c r="H2" t="n">
-        <v>0.641384018042984</v>
+        <v>3800114.19578297</v>
       </c>
       <c r="I2" t="n">
-        <v>0.646212530234465</v>
+        <v>3961001.32036821</v>
       </c>
       <c r="J2" t="n">
-        <v>0.654297128203085</v>
+        <v>3921480.68939769</v>
       </c>
       <c r="K2" t="n">
-        <v>0.659584872840855</v>
+        <v>4018540.51467808</v>
       </c>
       <c r="L2" t="n">
-        <v>0.646090143119001</v>
+        <v>3958881.62889474</v>
       </c>
       <c r="M2" t="n">
-        <v>0.658736111789436</v>
+        <v>3999440.05047612</v>
       </c>
     </row>
     <row r="3">
@@ -481,16 +481,16 @@
         <v>14</v>
       </c>
       <c r="B3" t="n">
-        <v>0.00396034612901532</v>
+        <v>24166.248</v>
       </c>
       <c r="C3" t="n">
-        <v>0.00643091300292547</v>
+        <v>39349.2212</v>
       </c>
       <c r="D3" t="n">
-        <v>0.00481374953406502</v>
+        <v>20463.548</v>
       </c>
       <c r="E3" t="n">
-        <v>0.00231016719790819</v>
+        <v>13056.9402</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -522,40 +522,40 @@
         <v>15</v>
       </c>
       <c r="B4" t="n">
-        <v>0.333785990652592</v>
+        <v>2036780.3132</v>
       </c>
       <c r="C4" t="n">
-        <v>0.316436886723438</v>
+        <v>1936201.7564</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0659985263709172</v>
+        <v>280563.831325896</v>
       </c>
       <c r="E4" t="n">
-        <v>0.34913288148633</v>
+        <v>1973280.18489243</v>
       </c>
       <c r="F4" t="n">
-        <v>0.334172971390928</v>
+        <v>1979415.55517132</v>
       </c>
       <c r="G4" t="n">
-        <v>0.293870504463264</v>
+        <v>2017091.71892112</v>
       </c>
       <c r="H4" t="n">
-        <v>0.358615981957016</v>
+        <v>2124751.54592669</v>
       </c>
       <c r="I4" t="n">
-        <v>0.353787469765535</v>
+        <v>2168563.07995538</v>
       </c>
       <c r="J4" t="n">
-        <v>0.345702871796915</v>
+        <v>2071944.19413705</v>
       </c>
       <c r="K4" t="n">
-        <v>0.340415127159145</v>
+        <v>2073989.31756335</v>
       </c>
       <c r="L4" t="n">
-        <v>0.353909856880999</v>
+        <v>2168563.07995538</v>
       </c>
       <c r="M4" t="n">
-        <v>0.341263888210564</v>
+        <v>2071944.19413705</v>
       </c>
     </row>
     <row r="5">
@@ -563,16 +563,16 @@
         <v>16</v>
       </c>
       <c r="B5" t="n">
-        <v>0.00396034612901532</v>
+        <v>24166.248</v>
       </c>
       <c r="C5" t="n">
-        <v>0.00643091300292547</v>
+        <v>39349.2212</v>
       </c>
       <c r="D5" t="n">
-        <v>0.00481374953406502</v>
+        <v>20463.548</v>
       </c>
       <c r="E5" t="n">
-        <v>0.00231016719790819</v>
+        <v>13056.9402</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>

</xml_diff>